<commit_message>
created comp data object, populated drivers & assumptions accordingly
</commit_message>
<xml_diff>
--- a/lib/CompCompCalc_formula.xlsx
+++ b/lib/CompCompCalc_formula.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Drivers" sheetId="1" r:id="rId1"/>
-    <sheet name="Equity Valuation" sheetId="2" r:id="rId2"/>
+    <sheet name="Equity Valuation" sheetId="2" r:id="rId1"/>
+    <sheet name="Drivers" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -53,15 +53,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>Salary</t>
   </si>
   <si>
     <t>weighted value</t>
-  </si>
-  <si>
-    <t>Bonus</t>
   </si>
   <si>
     <t>Vacation</t>
@@ -336,6 +333,15 @@
   <si>
     <t>see likelihood</t>
   </si>
+  <si>
+    <t>Annual Bonus</t>
+  </si>
+  <si>
+    <t>Signing Bonus</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
 </sst>
 </file>
 
@@ -359,7 +365,7 @@
     <numFmt numFmtId="176" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="178" formatCode="0%\ &quot; will vest&quot;"/>
-    <numFmt numFmtId="180" formatCode="0%\ &quot; chance hit target&quot;"/>
+    <numFmt numFmtId="179" formatCode="0%\ &quot; chance hit target&quot;"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -691,7 +697,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -885,8 +891,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -939,8 +943,6 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,7 +968,7 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="23" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="23" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -988,6 +990,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="23" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1125,7 +1138,7 @@
             <c:numRef>
               <c:f>[1]USA!$J$6:$J$19</c:f>
               <c:numCache>
-                <c:formatCode>"$"#,##0;[Red]\-"$"#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>137568</c:v>
@@ -1258,7 +1271,7 @@
             <c:numRef>
               <c:f>[1]USA!$K$6:$K$19</c:f>
               <c:numCache>
-                <c:formatCode>"$"#,##0;[Red]\-"$"#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>187248.0</c:v>
@@ -1327,11 +1340,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1596998576"/>
-        <c:axId val="-1529165264"/>
+        <c:axId val="-833580400"/>
+        <c:axId val="-836458560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1596998576"/>
+        <c:axId val="-833580400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1370,7 +1383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1529165264"/>
+        <c:crossAx val="-836458560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1378,7 +1391,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1529165264"/>
+        <c:axId val="-836458560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1412,7 +1425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1596998576"/>
+        <c:crossAx val="-833580400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1912,897 +1925,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="1" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="133"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="43"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="134"/>
-      <c r="G2" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="43"/>
-    </row>
-    <row r="3" spans="1:17" s="7" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="135"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="46">
-        <f>SUM(K4:K18)</f>
-        <v>207823.46153846153</v>
-      </c>
-      <c r="L3" s="46">
-        <f>SUM(L4:L18)</f>
-        <v>300516.15384615387</v>
-      </c>
-      <c r="M3" s="48"/>
-      <c r="N3" s="52">
-        <f>SUM(N4:N22)</f>
-        <v>108300</v>
-      </c>
-      <c r="O3" s="13">
-        <f>SUM(O4:O22)</f>
-        <v>300516.15384615387</v>
-      </c>
-      <c r="P3" s="13">
-        <f>SUM(P4:P22)</f>
-        <v>492183.07692307694</v>
-      </c>
-      <c r="Q3" s="44"/>
-    </row>
-    <row r="4" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="70">
-        <f>L4</f>
-        <v>92000</v>
-      </c>
-      <c r="E4" s="33">
-        <v>1</v>
-      </c>
-      <c r="F4" s="136"/>
-      <c r="G4" s="36">
-        <v>75000</v>
-      </c>
-      <c r="H4" s="65">
-        <v>92000</v>
-      </c>
-      <c r="I4" s="15">
-        <v>95000</v>
-      </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="35">
-        <f>L4*E4</f>
-        <v>92000</v>
-      </c>
-      <c r="L4" s="34">
-        <f>H4/E4</f>
-        <v>92000</v>
-      </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="41">
-        <f>O4</f>
-        <v>92000</v>
-      </c>
-      <c r="O4" s="14">
-        <f>L4</f>
-        <v>92000</v>
-      </c>
-      <c r="P4" s="9">
-        <f>O4</f>
-        <v>92000</v>
-      </c>
-      <c r="Q4" s="43"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="70">
-        <f>L5</f>
-        <v>18000</v>
-      </c>
-      <c r="E5" s="132">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="136"/>
-      <c r="G5" s="37">
-        <v>10000</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="15">
-        <v>20000</v>
-      </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="35">
-        <f>L5*E5</f>
-        <v>14400</v>
-      </c>
-      <c r="L5" s="35">
-        <f>(I5-G5)*E5+G5</f>
-        <v>18000</v>
-      </c>
-      <c r="M5" s="30"/>
-      <c r="N5" s="42">
-        <f>G5</f>
-        <v>10000</v>
-      </c>
-      <c r="O5" s="14">
-        <f>L5</f>
-        <v>18000</v>
-      </c>
-      <c r="P5" s="9">
-        <f>I5</f>
-        <v>20000</v>
-      </c>
-      <c r="Q5" s="43"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="72">
-        <f>'Equity Valuation'!C26</f>
-        <v>24000</v>
-      </c>
-      <c r="E6" s="131">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="137"/>
-      <c r="G6" s="37">
-        <f>I6/4</f>
-        <v>36719.999999999993</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" s="15">
-        <f>'Equity Valuation'!J6</f>
-        <v>146879.99999999997</v>
-      </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="35">
-        <f>G6</f>
-        <v>36719.999999999993</v>
-      </c>
-      <c r="L6" s="35">
-        <f>I6*E6</f>
-        <v>73439.999999999985</v>
-      </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="42">
-        <v>0</v>
-      </c>
-      <c r="O6" s="14">
-        <f>L6</f>
-        <v>73439.999999999985</v>
-      </c>
-      <c r="P6" s="9">
-        <f>I6</f>
-        <v>146879.99999999997</v>
-      </c>
-      <c r="Q6" s="43"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="71">
-        <f>'Equity Valuation'!C29</f>
-        <v>24000</v>
-      </c>
-      <c r="E7" s="131">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="137"/>
-      <c r="G7" s="37">
-        <f>I7/4</f>
-        <v>49140</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="15">
-        <f>'Equity Valuation'!K6</f>
-        <v>196560</v>
-      </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="35">
-        <f>G7</f>
-        <v>49140</v>
-      </c>
-      <c r="L7" s="35">
-        <f>I7*E7</f>
-        <v>98280</v>
-      </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="42">
-        <v>0</v>
-      </c>
-      <c r="O7" s="14">
-        <f>L7</f>
-        <v>98280</v>
-      </c>
-      <c r="P7" s="9">
-        <f>I7</f>
-        <v>196560</v>
-      </c>
-      <c r="Q7" s="43"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="31">
-        <f>H8</f>
-        <v>3</v>
-      </c>
-      <c r="E8" s="32">
-        <v>0.66</v>
-      </c>
-      <c r="F8" s="138"/>
-      <c r="G8" s="38">
-        <v>2</v>
-      </c>
-      <c r="H8" s="22">
-        <v>3</v>
-      </c>
-      <c r="I8" s="21">
-        <v>6</v>
-      </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="35">
-        <f>L8*E8</f>
-        <v>4188.4615384615381</v>
-      </c>
-      <c r="L8" s="35">
-        <f>(L4+L5)/52*H8</f>
-        <v>6346.1538461538457</v>
-      </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="42">
-        <v>0</v>
-      </c>
-      <c r="O8" s="14">
-        <f>L8</f>
-        <v>6346.1538461538457</v>
-      </c>
-      <c r="P8" s="9">
-        <f>D4/52*H8</f>
-        <v>5307.6923076923076</v>
-      </c>
-      <c r="Q8" s="43"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="70">
-        <f>H9</f>
-        <v>500</v>
-      </c>
-      <c r="E9" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="138"/>
-      <c r="G9" s="64">
-        <v>400</v>
-      </c>
-      <c r="H9" s="65">
-        <v>500</v>
-      </c>
-      <c r="I9" s="66">
-        <v>600</v>
-      </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="35">
-        <f>L9*E9</f>
-        <v>125</v>
-      </c>
-      <c r="L9" s="35">
-        <f>O9</f>
-        <v>250</v>
-      </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="42">
-        <f>G9*E9</f>
-        <v>200</v>
-      </c>
-      <c r="O9" s="9">
-        <f>H9*E$9</f>
-        <v>250</v>
-      </c>
-      <c r="P9" s="9">
-        <f>I9*E9</f>
-        <v>300</v>
-      </c>
-      <c r="Q9" s="43"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="70">
-        <f>H10</f>
-        <v>2000</v>
-      </c>
-      <c r="E10" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="138"/>
-      <c r="G10" s="64">
-        <v>1000</v>
-      </c>
-      <c r="H10" s="65">
-        <v>2000</v>
-      </c>
-      <c r="I10" s="66">
-        <v>3000</v>
-      </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="35">
-        <f>L10*E10</f>
-        <v>500</v>
-      </c>
-      <c r="L10" s="35">
-        <f>O10</f>
-        <v>1000</v>
-      </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="42">
-        <f>G10*E10</f>
-        <v>500</v>
-      </c>
-      <c r="O10" s="9">
-        <f>H10*E$9</f>
-        <v>1000</v>
-      </c>
-      <c r="P10" s="9">
-        <f>I10*E10</f>
-        <v>1500</v>
-      </c>
-      <c r="Q10" s="43"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="70">
-        <f>H11</f>
-        <v>1800</v>
-      </c>
-      <c r="E11" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="138"/>
-      <c r="G11" s="64">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="65">
-        <v>1800</v>
-      </c>
-      <c r="I11" s="66">
-        <v>3000</v>
-      </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="35">
-        <f>L11*E11</f>
-        <v>450</v>
-      </c>
-      <c r="L11" s="35">
-        <f>O11</f>
-        <v>900</v>
-      </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="42">
-        <f>G11*E11</f>
-        <v>500</v>
-      </c>
-      <c r="O11" s="9">
-        <f>H11*E$9</f>
-        <v>900</v>
-      </c>
-      <c r="P11" s="9">
-        <f>I11*E11</f>
-        <v>1500</v>
-      </c>
-      <c r="Q11" s="43"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="70">
-        <f>K12</f>
-        <v>4600</v>
-      </c>
-      <c r="E12" s="32">
-        <v>1</v>
-      </c>
-      <c r="F12" s="133"/>
-      <c r="G12" s="39">
-        <v>0</v>
-      </c>
-      <c r="H12" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I12" s="23">
-        <v>0.06</v>
-      </c>
-      <c r="J12" s="30"/>
-      <c r="K12" s="35">
-        <f>L12*E12</f>
-        <v>4600</v>
-      </c>
-      <c r="L12" s="35">
-        <f>O12</f>
-        <v>4600</v>
-      </c>
-      <c r="M12" s="30"/>
-      <c r="N12" s="42">
-        <f>$D$4*G12</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="9">
-        <f>$D$4*H12</f>
-        <v>4600</v>
-      </c>
-      <c r="P12" s="9">
-        <f>$D$4*I12</f>
-        <v>5520</v>
-      </c>
-      <c r="Q12" s="43"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="139">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="32">
-        <v>1</v>
-      </c>
-      <c r="F13" s="133"/>
-      <c r="G13" s="40">
-        <v>400</v>
-      </c>
-      <c r="H13" s="26">
-        <v>550</v>
-      </c>
-      <c r="I13" s="25">
-        <v>800</v>
-      </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="35">
-        <f>L13*E13</f>
-        <v>3300</v>
-      </c>
-      <c r="L13" s="35">
-        <f>O13</f>
-        <v>3300</v>
-      </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="42">
-        <f>G13*12*$D$13</f>
-        <v>2400</v>
-      </c>
-      <c r="O13" s="9">
-        <f>H13*12*$D$13</f>
-        <v>3300</v>
-      </c>
-      <c r="P13" s="9">
-        <f>I13*12*$D$13</f>
-        <v>4800</v>
-      </c>
-      <c r="Q13" s="43"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="70">
-        <f>H14</f>
-        <v>75</v>
-      </c>
-      <c r="E14" s="32">
-        <v>1</v>
-      </c>
-      <c r="F14" s="133"/>
-      <c r="G14" s="67">
-        <v>50</v>
-      </c>
-      <c r="H14" s="68">
-        <v>75</v>
-      </c>
-      <c r="I14" s="69">
-        <v>100</v>
-      </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="35">
-        <f>L14*E14</f>
-        <v>450</v>
-      </c>
-      <c r="L14" s="35">
-        <f>O14</f>
-        <v>450</v>
-      </c>
-      <c r="M14" s="30"/>
-      <c r="N14" s="42">
-        <f>G14*E14*12</f>
-        <v>600</v>
-      </c>
-      <c r="O14" s="9">
-        <f>H14*E$9*12</f>
-        <v>450</v>
-      </c>
-      <c r="P14" s="9">
-        <f>I14*E14*12</f>
-        <v>1200</v>
-      </c>
-      <c r="Q14" s="43"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="70">
-        <f>H15</f>
-        <v>125</v>
-      </c>
-      <c r="E15" s="32">
-        <v>1</v>
-      </c>
-      <c r="F15" s="133"/>
-      <c r="G15" s="67">
-        <v>75</v>
-      </c>
-      <c r="H15" s="68">
-        <v>125</v>
-      </c>
-      <c r="I15" s="69">
-        <v>200</v>
-      </c>
-      <c r="J15" s="30"/>
-      <c r="K15" s="35">
-        <f>L15*E15</f>
-        <v>750</v>
-      </c>
-      <c r="L15" s="35">
-        <f>O15</f>
-        <v>750</v>
-      </c>
-      <c r="M15" s="30"/>
-      <c r="N15" s="42">
-        <f>G15*E15*12</f>
-        <v>900</v>
-      </c>
-      <c r="O15" s="9">
-        <f>H15*E$9*12</f>
-        <v>750</v>
-      </c>
-      <c r="P15" s="9">
-        <f>I15*E15*12</f>
-        <v>2400</v>
-      </c>
-      <c r="Q15" s="43"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="70">
-        <f>H16</f>
-        <v>200</v>
-      </c>
-      <c r="E16" s="32">
-        <v>1</v>
-      </c>
-      <c r="F16" s="133"/>
-      <c r="G16" s="67">
-        <v>100</v>
-      </c>
-      <c r="H16" s="68">
-        <v>200</v>
-      </c>
-      <c r="I16" s="69">
-        <v>300</v>
-      </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="35">
-        <f>L16*E16</f>
-        <v>1200</v>
-      </c>
-      <c r="L16" s="35">
-        <f>O16</f>
-        <v>1200</v>
-      </c>
-      <c r="M16" s="30"/>
-      <c r="N16" s="42">
-        <f>G16*E16*12</f>
-        <v>1200</v>
-      </c>
-      <c r="O16" s="9">
-        <f>H16*E$9*12</f>
-        <v>1200</v>
-      </c>
-      <c r="P16" s="9">
-        <f>I16*E16*12</f>
-        <v>3600</v>
-      </c>
-      <c r="Q16" s="43"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="31">
-        <f>H17</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="32">
-        <v>0</v>
-      </c>
-      <c r="F17" s="138"/>
-      <c r="G17" s="38">
-        <v>0</v>
-      </c>
-      <c r="H17" s="22">
-        <f>I17*E17</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="21">
-        <v>6</v>
-      </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="35">
-        <f>L17*E17</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="35">
-        <f>O17</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="30"/>
-      <c r="N17" s="42">
-        <f>$H$4/52*G17</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="14">
-        <f>$H$4/52*H17</f>
-        <v>0</v>
-      </c>
-      <c r="P17" s="9">
-        <f>$H$4/52*I17</f>
-        <v>10615.384615384615</v>
-      </c>
-      <c r="Q17" s="43"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="F18" s="133"/>
-      <c r="G18" s="64">
-        <v>0</v>
-      </c>
-      <c r="H18" s="65">
-        <v>0</v>
-      </c>
-      <c r="I18" s="66">
-        <v>0</v>
-      </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="35">
-        <f>L18*E18</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="35">
-        <f>H18</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="30"/>
-      <c r="N18" s="42">
-        <f>G18</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="9">
-        <f>H18</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="9">
-        <f>I18</f>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="43"/>
-    </row>
-    <row r="19" spans="1:17" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="63"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="43"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="E22" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1005"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2860,12 +1987,12 @@
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="73"/>
       <c r="B2" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="77" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="78"/>
+        <v>37</v>
+      </c>
+      <c r="C2" s="136" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="137"/>
       <c r="E2" s="74"/>
       <c r="F2" s="76"/>
       <c r="G2" s="76"/>
@@ -2898,7 +2025,7 @@
       <c r="E3" s="74"/>
       <c r="F3" s="76"/>
       <c r="G3" s="76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="73"/>
       <c r="J3" s="73"/>
@@ -2923,34 +2050,34 @@
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="81" t="s">
+      <c r="G4" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="82" t="s">
+      <c r="H4" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="82" t="s">
+      <c r="I4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="82" t="s">
+      <c r="J4" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="K4" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="L4" s="80" t="s">
         <v>47</v>
-      </c>
-      <c r="L4" s="82" t="s">
-        <v>48</v>
       </c>
       <c r="M4" s="74"/>
       <c r="N4" s="73"/>
@@ -2974,32 +2101,32 @@
       <c r="B5" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="81">
         <v>0</v>
       </c>
       <c r="D5" s="73"/>
       <c r="E5" s="74"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84" t="str">
+      <c r="F5" s="82"/>
+      <c r="G5" s="82" t="str">
         <f t="shared" ref="G5:G18" si="0">"$"&amp;H5/1000000000&amp;"B"</f>
         <v>$2B</v>
       </c>
-      <c r="H5" s="85">
+      <c r="H5" s="83">
         <f>C24</f>
         <v>2000000000</v>
       </c>
-      <c r="I5" s="86">
+      <c r="I5" s="84">
         <v>7.8019999999999996</v>
       </c>
-      <c r="J5" s="85">
+      <c r="J5" s="83">
         <f t="shared" ref="J5:J18" si="1">(I5-$C$23)*$C$26</f>
         <v>137567.99999999997</v>
       </c>
-      <c r="K5" s="85">
+      <c r="K5" s="83">
         <f t="shared" ref="K5:K18" si="2">I5*$C$29</f>
         <v>187248</v>
       </c>
-      <c r="L5" s="85">
+      <c r="L5" s="83">
         <f t="shared" ref="L5:L18" si="3">J5+K5</f>
         <v>324816</v>
       </c>
@@ -3023,34 +2150,34 @@
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="73"/>
       <c r="B6" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="83">
+        <v>48</v>
+      </c>
+      <c r="C6" s="81">
         <f>C5*0.08</f>
         <v>0</v>
       </c>
-      <c r="D6" s="87"/>
+      <c r="D6" s="85"/>
       <c r="E6" s="74"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84" t="str">
+      <c r="F6" s="82"/>
+      <c r="G6" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$3B</v>
       </c>
-      <c r="H6" s="85">
+      <c r="H6" s="83">
         <v>3000000000</v>
       </c>
-      <c r="I6" s="86">
+      <c r="I6" s="84">
         <v>8.19</v>
       </c>
-      <c r="J6" s="85">
+      <c r="J6" s="83">
         <f t="shared" si="1"/>
         <v>146879.99999999997</v>
       </c>
-      <c r="K6" s="85">
+      <c r="K6" s="83">
         <f t="shared" si="2"/>
         <v>196560</v>
       </c>
-      <c r="L6" s="85">
+      <c r="L6" s="83">
         <f t="shared" si="3"/>
         <v>343440</v>
       </c>
@@ -3074,36 +2201,36 @@
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="73"/>
       <c r="B7" s="73" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="85">
+        <v>49</v>
+      </c>
+      <c r="C7" s="83">
         <v>0</v>
       </c>
       <c r="D7" s="73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="74"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84" t="str">
+      <c r="F7" s="82"/>
+      <c r="G7" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$5B</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="83">
         <f>H6+2000000000</f>
         <v>5000000000</v>
       </c>
-      <c r="I7" s="86">
+      <c r="I7" s="84">
         <v>10.24</v>
       </c>
-      <c r="J7" s="85">
+      <c r="J7" s="83">
         <f t="shared" si="1"/>
         <v>196080</v>
       </c>
-      <c r="K7" s="85">
+      <c r="K7" s="83">
         <f t="shared" si="2"/>
         <v>245760</v>
       </c>
-      <c r="L7" s="85">
+      <c r="L7" s="83">
         <f t="shared" si="3"/>
         <v>441840</v>
       </c>
@@ -3127,36 +2254,36 @@
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="73"/>
       <c r="B8" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="85">
+        <v>25</v>
+      </c>
+      <c r="C8" s="83">
         <v>0</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="74"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84" t="str">
+      <c r="F8" s="82"/>
+      <c r="G8" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$10B</v>
       </c>
-      <c r="H8" s="85">
+      <c r="H8" s="83">
         <f t="shared" ref="H8:H16" si="4">H7+5000000000</f>
         <v>10000000000</v>
       </c>
-      <c r="I8" s="86">
+      <c r="I8" s="84">
         <v>20.49</v>
       </c>
-      <c r="J8" s="85">
+      <c r="J8" s="83">
         <f t="shared" si="1"/>
         <v>442079.99999999994</v>
       </c>
-      <c r="K8" s="85">
+      <c r="K8" s="83">
         <f t="shared" si="2"/>
         <v>491759.99999999994</v>
       </c>
-      <c r="L8" s="85">
+      <c r="L8" s="83">
         <f t="shared" si="3"/>
         <v>933839.99999999988</v>
       </c>
@@ -3180,36 +2307,36 @@
     <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="73"/>
       <c r="B9" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="85">
+        <v>26</v>
+      </c>
+      <c r="C9" s="83">
         <v>0</v>
       </c>
       <c r="D9" s="73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="74"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84" t="str">
+      <c r="F9" s="82"/>
+      <c r="G9" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$15B</v>
       </c>
-      <c r="H9" s="85">
+      <c r="H9" s="83">
         <f t="shared" si="4"/>
         <v>15000000000</v>
       </c>
-      <c r="I9" s="86">
+      <c r="I9" s="84">
         <v>30.73</v>
       </c>
-      <c r="J9" s="85">
+      <c r="J9" s="83">
         <f t="shared" si="1"/>
         <v>687840</v>
       </c>
-      <c r="K9" s="85">
+      <c r="K9" s="83">
         <f t="shared" si="2"/>
         <v>737520</v>
       </c>
-      <c r="L9" s="85">
+      <c r="L9" s="83">
         <f t="shared" si="3"/>
         <v>1425360</v>
       </c>
@@ -3233,34 +2360,34 @@
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="73"/>
       <c r="B10" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="85">
+        <v>50</v>
+      </c>
+      <c r="C10" s="83">
         <v>0</v>
       </c>
       <c r="D10" s="73"/>
       <c r="E10" s="74"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84" t="str">
+      <c r="F10" s="82"/>
+      <c r="G10" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$20B</v>
       </c>
-      <c r="H10" s="85">
+      <c r="H10" s="83">
         <f t="shared" si="4"/>
         <v>20000000000</v>
       </c>
-      <c r="I10" s="86">
+      <c r="I10" s="84">
         <v>40.97</v>
       </c>
-      <c r="J10" s="85">
+      <c r="J10" s="83">
         <f t="shared" si="1"/>
         <v>933600</v>
       </c>
-      <c r="K10" s="85">
+      <c r="K10" s="83">
         <f t="shared" si="2"/>
         <v>983280</v>
       </c>
-      <c r="L10" s="85">
+      <c r="L10" s="83">
         <f t="shared" si="3"/>
         <v>1916880</v>
       </c>
@@ -3284,34 +2411,34 @@
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="73"/>
       <c r="B11" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="85">
+        <v>51</v>
+      </c>
+      <c r="C11" s="83">
         <v>0</v>
       </c>
       <c r="D11" s="73"/>
       <c r="E11" s="74"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84" t="str">
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$25B</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="83">
         <f t="shared" si="4"/>
         <v>25000000000</v>
       </c>
-      <c r="I11" s="86">
+      <c r="I11" s="84">
         <v>51.22</v>
       </c>
-      <c r="J11" s="85">
+      <c r="J11" s="83">
         <f t="shared" si="1"/>
         <v>1179600</v>
       </c>
-      <c r="K11" s="85">
+      <c r="K11" s="83">
         <f t="shared" si="2"/>
         <v>1229280</v>
       </c>
-      <c r="L11" s="85">
+      <c r="L11" s="83">
         <f t="shared" si="3"/>
         <v>2408880</v>
       </c>
@@ -3335,34 +2462,34 @@
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="73"/>
       <c r="B12" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="85">
+        <v>52</v>
+      </c>
+      <c r="C12" s="83">
         <v>0</v>
       </c>
       <c r="D12" s="73"/>
       <c r="E12" s="74"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84" t="str">
+      <c r="F12" s="82"/>
+      <c r="G12" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$30B</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="83">
         <f t="shared" si="4"/>
         <v>30000000000</v>
       </c>
-      <c r="I12" s="86">
+      <c r="I12" s="84">
         <v>61.46</v>
       </c>
-      <c r="J12" s="85">
+      <c r="J12" s="83">
         <f t="shared" si="1"/>
         <v>1425360</v>
       </c>
-      <c r="K12" s="85">
+      <c r="K12" s="83">
         <f t="shared" si="2"/>
         <v>1475040</v>
       </c>
-      <c r="L12" s="85">
+      <c r="L12" s="83">
         <f t="shared" si="3"/>
         <v>2900400</v>
       </c>
@@ -3385,35 +2512,35 @@
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="73"/>
-      <c r="B13" s="88" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="89">
+      <c r="B13" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="87">
         <v>0</v>
       </c>
-      <c r="D13" s="90"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="74"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84" t="str">
+      <c r="F13" s="82"/>
+      <c r="G13" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$35B</v>
       </c>
-      <c r="H13" s="85">
+      <c r="H13" s="83">
         <f t="shared" si="4"/>
         <v>35000000000</v>
       </c>
-      <c r="I13" s="86">
+      <c r="I13" s="84">
         <v>71.709999999999994</v>
       </c>
-      <c r="J13" s="85">
+      <c r="J13" s="83">
         <f t="shared" si="1"/>
         <v>1671360</v>
       </c>
-      <c r="K13" s="85">
+      <c r="K13" s="83">
         <f t="shared" si="2"/>
         <v>1721039.9999999998</v>
       </c>
-      <c r="L13" s="85">
+      <c r="L13" s="83">
         <f t="shared" si="3"/>
         <v>3392400</v>
       </c>
@@ -3436,36 +2563,36 @@
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="73"/>
-      <c r="B14" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="92">
+      <c r="B14" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="90">
         <f>SUM(C5:C13)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="93"/>
+      <c r="D14" s="91"/>
       <c r="E14" s="74"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84" t="str">
+      <c r="F14" s="82"/>
+      <c r="G14" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$40B</v>
       </c>
-      <c r="H14" s="85">
+      <c r="H14" s="83">
         <f t="shared" si="4"/>
         <v>40000000000</v>
       </c>
-      <c r="I14" s="86">
+      <c r="I14" s="84">
         <v>81.95</v>
       </c>
-      <c r="J14" s="85">
+      <c r="J14" s="83">
         <f t="shared" si="1"/>
         <v>1917120.0000000002</v>
       </c>
-      <c r="K14" s="85">
+      <c r="K14" s="83">
         <f t="shared" si="2"/>
         <v>1966800</v>
       </c>
-      <c r="L14" s="85">
+      <c r="L14" s="83">
         <f t="shared" si="3"/>
         <v>3883920</v>
       </c>
@@ -3492,27 +2619,27 @@
       <c r="C15" s="73"/>
       <c r="D15" s="73"/>
       <c r="E15" s="74"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84" t="str">
+      <c r="F15" s="82"/>
+      <c r="G15" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$45B</v>
       </c>
-      <c r="H15" s="85">
+      <c r="H15" s="83">
         <f t="shared" si="4"/>
         <v>45000000000</v>
       </c>
-      <c r="I15" s="86">
+      <c r="I15" s="84">
         <v>92.19</v>
       </c>
-      <c r="J15" s="85">
+      <c r="J15" s="83">
         <f t="shared" si="1"/>
         <v>2162880</v>
       </c>
-      <c r="K15" s="85">
+      <c r="K15" s="83">
         <f t="shared" si="2"/>
         <v>2212560</v>
       </c>
-      <c r="L15" s="85">
+      <c r="L15" s="83">
         <f t="shared" si="3"/>
         <v>4375440</v>
       </c>
@@ -3535,35 +2662,35 @@
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="96"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="94"/>
       <c r="E16" s="74"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84" t="str">
+      <c r="F16" s="82"/>
+      <c r="G16" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$50B</v>
       </c>
-      <c r="H16" s="85">
+      <c r="H16" s="83">
         <f t="shared" si="4"/>
         <v>50000000000</v>
       </c>
-      <c r="I16" s="86">
+      <c r="I16" s="84">
         <v>102.44</v>
       </c>
-      <c r="J16" s="85">
+      <c r="J16" s="83">
         <f t="shared" si="1"/>
         <v>2408880</v>
       </c>
-      <c r="K16" s="85">
+      <c r="K16" s="83">
         <f t="shared" si="2"/>
         <v>2458560</v>
       </c>
-      <c r="L16" s="85">
+      <c r="L16" s="83">
         <f t="shared" si="3"/>
         <v>4867440</v>
       </c>
@@ -3587,34 +2714,34 @@
     <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="73"/>
       <c r="B17" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="73" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>59</v>
       </c>
       <c r="D17" s="73"/>
       <c r="E17" s="74"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84" t="str">
+      <c r="F17" s="82"/>
+      <c r="G17" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$75B</v>
       </c>
-      <c r="H17" s="85">
+      <c r="H17" s="83">
         <f t="shared" ref="H17:H18" si="5">H16+25000000000</f>
         <v>75000000000</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="84">
         <v>153.66</v>
       </c>
-      <c r="J17" s="85">
+      <c r="J17" s="83">
         <f t="shared" si="1"/>
         <v>3638160</v>
       </c>
-      <c r="K17" s="85">
+      <c r="K17" s="83">
         <f t="shared" si="2"/>
         <v>3687840</v>
       </c>
-      <c r="L17" s="85">
+      <c r="L17" s="83">
         <f t="shared" si="3"/>
         <v>7326000</v>
       </c>
@@ -3638,34 +2765,34 @@
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="73"/>
       <c r="B18" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="73" t="s">
         <v>60</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>61</v>
       </c>
       <c r="D18" s="73"/>
       <c r="E18" s="74"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84" t="str">
+      <c r="F18" s="82"/>
+      <c r="G18" s="82" t="str">
         <f t="shared" si="0"/>
         <v>$100B</v>
       </c>
-      <c r="H18" s="85">
+      <c r="H18" s="83">
         <f t="shared" si="5"/>
         <v>100000000000</v>
       </c>
-      <c r="I18" s="86">
+      <c r="I18" s="84">
         <v>204.87</v>
       </c>
-      <c r="J18" s="85">
+      <c r="J18" s="83">
         <f t="shared" si="1"/>
         <v>4867200</v>
       </c>
-      <c r="K18" s="85">
+      <c r="K18" s="83">
         <f t="shared" si="2"/>
         <v>4916880</v>
       </c>
-      <c r="L18" s="85">
+      <c r="L18" s="83">
         <f t="shared" si="3"/>
         <v>9784080</v>
       </c>
@@ -3689,22 +2816,22 @@
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="73"/>
       <c r="B19" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="73" t="s">
         <v>62</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>63</v>
       </c>
       <c r="D19" s="73"/>
       <c r="E19" s="74"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="97" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="93"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="95" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="91"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="91"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="91"/>
       <c r="M19" s="74"/>
       <c r="N19" s="73"/>
       <c r="O19" s="73"/>
@@ -3724,34 +2851,34 @@
     </row>
     <row r="20" spans="1:28" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="73"/>
-      <c r="B20" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="99">
+      <c r="B20" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="97">
         <f>I20</f>
         <v>461423849</v>
       </c>
-      <c r="D20" s="100"/>
-      <c r="E20" s="101"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="99"/>
       <c r="F20" s="73"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="102" t="s">
+      <c r="G20" s="100"/>
+      <c r="H20" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="101">
+        <v>461423849</v>
+      </c>
+      <c r="J20" s="98"/>
+      <c r="K20" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="I20" s="103">
-        <v>461423849</v>
-      </c>
-      <c r="J20" s="100"/>
-      <c r="K20" s="104" t="s">
-        <v>67</v>
-      </c>
-      <c r="L20" s="100"/>
+      <c r="L20" s="98"/>
       <c r="M20" s="74"/>
-      <c r="N20" s="105"/>
-      <c r="O20" s="105"/>
-      <c r="P20" s="105"/>
-      <c r="Q20" s="105"/>
-      <c r="R20" s="105"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="103"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="103"/>
       <c r="S20" s="74"/>
       <c r="T20" s="74"/>
       <c r="U20" s="74"/>
@@ -3765,13 +2892,13 @@
     </row>
     <row r="21" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="73"/>
-      <c r="F21" s="106"/>
+      <c r="F21" s="104"/>
       <c r="M21" s="74"/>
-      <c r="N21" s="85"/>
-      <c r="O21" s="86"/>
-      <c r="P21" s="86"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="85"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="84"/>
+      <c r="P21" s="84"/>
+      <c r="Q21" s="105"/>
+      <c r="R21" s="83"/>
       <c r="S21" s="74"/>
       <c r="T21" s="74"/>
       <c r="U21" s="74"/>
@@ -3786,12 +2913,12 @@
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="73"/>
       <c r="B22" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="108">
+        <v>67</v>
+      </c>
+      <c r="C22" s="106">
         <v>7.8019999999999996</v>
       </c>
-      <c r="D22" s="108"/>
+      <c r="D22" s="106"/>
       <c r="E22" s="74"/>
       <c r="F22" s="73"/>
       <c r="G22" s="73"/>
@@ -3801,11 +2928,11 @@
       <c r="K22" s="73"/>
       <c r="L22" s="73"/>
       <c r="M22" s="74"/>
-      <c r="N22" s="85"/>
-      <c r="O22" s="86"/>
-      <c r="P22" s="86"/>
-      <c r="Q22" s="107"/>
-      <c r="R22" s="85"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="105"/>
+      <c r="R22" s="83"/>
       <c r="S22" s="74"/>
       <c r="T22" s="74"/>
       <c r="U22" s="74"/>
@@ -3820,12 +2947,12 @@
     <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="73"/>
       <c r="B23" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="86">
+        <v>68</v>
+      </c>
+      <c r="C23" s="84">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D23" s="108"/>
+      <c r="D23" s="106"/>
       <c r="E23" s="74"/>
       <c r="F23" s="73"/>
       <c r="G23" s="73"/>
@@ -3854,24 +2981,24 @@
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="73"/>
       <c r="B24" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="83">
+        <v>2000000000</v>
+      </c>
+      <c r="D24" s="106"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="85">
-        <v>2000000000</v>
-      </c>
-      <c r="D24" s="108"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="81" t="s">
+      <c r="G24" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="109" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="110"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="112"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="110"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="110"/>
+      <c r="K24" s="110"/>
+      <c r="L24" s="108"/>
       <c r="M24" s="74"/>
       <c r="N24" s="73"/>
       <c r="O24" s="73"/>
@@ -3898,10 +3025,10 @@
       <c r="F25" s="73"/>
       <c r="G25" s="73"/>
       <c r="H25" s="73"/>
-      <c r="I25" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="J25" s="85">
+      <c r="I25" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="J25" s="83">
         <f>C14+(C33/4)</f>
         <v>81204</v>
       </c>
@@ -3927,21 +3054,21 @@
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="73"/>
       <c r="B26" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="113">
+        <v>73</v>
+      </c>
+      <c r="C26" s="111">
         <v>24000</v>
       </c>
-      <c r="D26" s="114">
+      <c r="D26" s="112">
         <v>8500</v>
       </c>
       <c r="F26" s="73"/>
       <c r="G26" s="73"/>
       <c r="H26" s="73"/>
-      <c r="I26" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" s="85">
+      <c r="I26" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" s="83">
         <f>J25*4</f>
         <v>324816</v>
       </c>
@@ -3967,9 +3094,9 @@
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="73"/>
       <c r="B27" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="85">
+        <v>75</v>
+      </c>
+      <c r="C27" s="83">
         <f>(C22-C23)*C26</f>
         <v>137567.99999999997</v>
       </c>
@@ -4001,14 +3128,14 @@
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="73"/>
       <c r="B28" s="73"/>
-      <c r="C28" s="114"/>
+      <c r="C28" s="140"/>
       <c r="D28" s="73"/>
       <c r="F28" s="73"/>
-      <c r="G28" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="H28" s="116"/>
-      <c r="I28" s="116"/>
+      <c r="G28" s="138" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="139"/>
+      <c r="I28" s="139"/>
       <c r="J28" s="73"/>
       <c r="K28" s="73"/>
       <c r="L28" s="73"/>
@@ -4032,12 +3159,12 @@
     <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="73"/>
       <c r="B29" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="113">
+        <v>77</v>
+      </c>
+      <c r="C29" s="111">
         <v>24000</v>
       </c>
-      <c r="D29" s="117">
+      <c r="D29" s="113">
         <v>9000</v>
       </c>
       <c r="E29" s="74"/>
@@ -4045,12 +3172,12 @@
       <c r="G29" s="73"/>
       <c r="H29" s="73"/>
       <c r="I29" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="J29" s="118" t="s">
-        <v>90</v>
-      </c>
-      <c r="K29" s="81"/>
+        <v>78</v>
+      </c>
+      <c r="J29" s="114" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" s="79"/>
       <c r="L29" s="73"/>
       <c r="M29" s="74"/>
       <c r="N29" s="73"/>
@@ -4072,13 +3199,13 @@
     <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="73"/>
       <c r="B30" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="85">
+        <v>79</v>
+      </c>
+      <c r="C30" s="83">
         <f>C22*C29</f>
         <v>187248</v>
       </c>
-      <c r="D30" s="119">
+      <c r="D30" s="115">
         <f>D26+D29</f>
         <v>17500</v>
       </c>
@@ -4086,17 +3213,17 @@
       <c r="F30" s="73"/>
       <c r="G30" s="73"/>
       <c r="H30" s="73"/>
-      <c r="I30" s="120" t="s">
-        <v>81</v>
-      </c>
-      <c r="J30" s="121">
+      <c r="I30" s="116" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="117">
         <f>VLOOKUP($J$29,$G$5:$L$19,6,FALSE)+(C14*4)</f>
         <v>343440</v>
       </c>
-      <c r="K30" s="120" t="s">
-        <v>82</v>
-      </c>
-      <c r="L30" s="121">
+      <c r="K30" s="116" t="s">
+        <v>81</v>
+      </c>
+      <c r="L30" s="117">
         <f>$J$30/4</f>
         <v>85860</v>
       </c>
@@ -4120,22 +3247,22 @@
       <c r="A31" s="73"/>
       <c r="B31" s="73"/>
       <c r="C31" s="73"/>
-      <c r="D31" s="122"/>
+      <c r="D31" s="118"/>
       <c r="E31" s="74"/>
       <c r="F31" s="73"/>
-      <c r="G31" s="123"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="91" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" s="124">
+      <c r="G31" s="119"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="J31" s="120">
         <f>VLOOKUP($J$29,$G$5:$L$19,6,FALSE)</f>
         <v>343440</v>
       </c>
-      <c r="K31" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="L31" s="124">
+      <c r="K31" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="L31" s="120">
         <f>$J$31/4</f>
         <v>85860</v>
       </c>
@@ -4157,15 +3284,15 @@
     </row>
     <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="73"/>
-      <c r="B32" s="120" t="s">
+      <c r="B32" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="121"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="123" t="s">
         <v>85</v>
-      </c>
-      <c r="C32" s="125"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="127" t="s">
-        <v>86</v>
       </c>
       <c r="H32" s="73"/>
       <c r="I32" s="73"/>
@@ -4191,18 +3318,18 @@
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="73"/>
-      <c r="B33" s="128" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="129">
+      <c r="B33" s="124" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="125">
         <f>C30+C27</f>
         <v>324816</v>
       </c>
-      <c r="D33" s="130"/>
+      <c r="D33" s="126"/>
       <c r="E33" s="74"/>
       <c r="F33" s="73"/>
-      <c r="G33" s="127" t="s">
-        <v>88</v>
+      <c r="G33" s="123" t="s">
+        <v>87</v>
       </c>
       <c r="H33" s="73"/>
       <c r="I33" s="73"/>
@@ -4421,11 +3548,11 @@
     <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="73"/>
       <c r="E41" s="74"/>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="81"/>
-      <c r="J41" s="81"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="79"/>
       <c r="K41" s="73"/>
       <c r="L41" s="73"/>
       <c r="M41" s="74"/>
@@ -4447,15 +3574,15 @@
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="73"/>
-      <c r="B42" s="85"/>
+      <c r="B42" s="83"/>
       <c r="C42" s="73"/>
       <c r="D42" s="73"/>
       <c r="E42" s="74"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
-      <c r="H42" s="85"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="85"/>
+      <c r="F42" s="83"/>
+      <c r="G42" s="83"/>
+      <c r="H42" s="83"/>
+      <c r="I42" s="83"/>
+      <c r="J42" s="83"/>
       <c r="K42" s="73"/>
       <c r="L42" s="73"/>
       <c r="M42" s="74"/>
@@ -4481,11 +3608,11 @@
       <c r="C43" s="73"/>
       <c r="D43" s="73"/>
       <c r="E43" s="74"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
-      <c r="H43" s="85"/>
-      <c r="I43" s="85"/>
-      <c r="J43" s="85"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
+      <c r="H43" s="83"/>
+      <c r="I43" s="83"/>
+      <c r="J43" s="83"/>
       <c r="K43" s="73"/>
       <c r="L43" s="73"/>
       <c r="M43" s="74"/>
@@ -4511,11 +3638,11 @@
       <c r="C44" s="73"/>
       <c r="D44" s="73"/>
       <c r="E44" s="74"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="85"/>
-      <c r="H44" s="85"/>
-      <c r="I44" s="85"/>
-      <c r="J44" s="85"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="83"/>
+      <c r="H44" s="83"/>
+      <c r="I44" s="83"/>
+      <c r="J44" s="83"/>
       <c r="K44" s="73"/>
       <c r="L44" s="73"/>
       <c r="M44" s="74"/>
@@ -4541,11 +3668,11 @@
       <c r="C45" s="73"/>
       <c r="D45" s="73"/>
       <c r="E45" s="74"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="83"/>
+      <c r="J45" s="83"/>
       <c r="K45" s="73"/>
       <c r="L45" s="73"/>
       <c r="M45" s="74"/>
@@ -4571,11 +3698,11 @@
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
       <c r="E46" s="74"/>
-      <c r="F46" s="85"/>
-      <c r="G46" s="85"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="85"/>
-      <c r="J46" s="85"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
       <c r="K46" s="73"/>
       <c r="L46" s="73"/>
       <c r="M46" s="74"/>
@@ -4601,11 +3728,11 @@
       <c r="C47" s="73"/>
       <c r="D47" s="73"/>
       <c r="E47" s="74"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
-      <c r="J47" s="85"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="83"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="83"/>
+      <c r="J47" s="83"/>
       <c r="K47" s="73"/>
       <c r="L47" s="73"/>
       <c r="M47" s="74"/>
@@ -4631,11 +3758,11 @@
       <c r="C48" s="73"/>
       <c r="D48" s="73"/>
       <c r="E48" s="74"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="83"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="83"/>
+      <c r="J48" s="83"/>
       <c r="K48" s="73"/>
       <c r="L48" s="73"/>
       <c r="M48" s="74"/>
@@ -4661,11 +3788,11 @@
       <c r="C49" s="73"/>
       <c r="D49" s="73"/>
       <c r="E49" s="74"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="85"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="83"/>
+      <c r="J49" s="83"/>
       <c r="K49" s="73"/>
       <c r="L49" s="73"/>
       <c r="M49" s="74"/>
@@ -4691,11 +3818,11 @@
       <c r="C50" s="73"/>
       <c r="D50" s="73"/>
       <c r="E50" s="74"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="85"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="83"/>
+      <c r="I50" s="83"/>
+      <c r="J50" s="83"/>
       <c r="K50" s="73"/>
       <c r="L50" s="73"/>
       <c r="M50" s="74"/>
@@ -4721,11 +3848,11 @@
       <c r="C51" s="73"/>
       <c r="D51" s="73"/>
       <c r="E51" s="74"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
-      <c r="H51" s="85"/>
-      <c r="I51" s="85"/>
-      <c r="J51" s="85"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
+      <c r="H51" s="83"/>
+      <c r="I51" s="83"/>
+      <c r="J51" s="83"/>
       <c r="K51" s="73"/>
       <c r="L51" s="73"/>
       <c r="M51" s="74"/>
@@ -4751,11 +3878,11 @@
       <c r="C52" s="73"/>
       <c r="D52" s="73"/>
       <c r="E52" s="74"/>
-      <c r="F52" s="85"/>
-      <c r="G52" s="85"/>
-      <c r="H52" s="85"/>
-      <c r="I52" s="85"/>
-      <c r="J52" s="85"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="83"/>
+      <c r="H52" s="83"/>
+      <c r="I52" s="83"/>
+      <c r="J52" s="83"/>
       <c r="K52" s="73"/>
       <c r="L52" s="73"/>
       <c r="M52" s="74"/>
@@ -4781,11 +3908,11 @@
       <c r="C53" s="73"/>
       <c r="D53" s="73"/>
       <c r="E53" s="74"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="85"/>
-      <c r="H53" s="85"/>
-      <c r="I53" s="85"/>
-      <c r="J53" s="85"/>
+      <c r="F53" s="83"/>
+      <c r="G53" s="83"/>
+      <c r="H53" s="83"/>
+      <c r="I53" s="83"/>
+      <c r="J53" s="83"/>
       <c r="K53" s="73"/>
       <c r="L53" s="73"/>
       <c r="M53" s="74"/>
@@ -4871,11 +3998,11 @@
       <c r="C56" s="73"/>
       <c r="D56" s="73"/>
       <c r="E56" s="73"/>
-      <c r="F56" s="105"/>
-      <c r="G56" s="105"/>
-      <c r="H56" s="105"/>
-      <c r="I56" s="105"/>
-      <c r="J56" s="105"/>
+      <c r="F56" s="103"/>
+      <c r="G56" s="103"/>
+      <c r="H56" s="103"/>
+      <c r="I56" s="103"/>
+      <c r="J56" s="103"/>
       <c r="K56" s="73"/>
       <c r="L56" s="73"/>
       <c r="M56" s="74"/>
@@ -4900,12 +4027,12 @@
       <c r="B57" s="73"/>
       <c r="C57" s="73"/>
       <c r="D57" s="73"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="85"/>
-      <c r="G57" s="85"/>
-      <c r="H57" s="85"/>
-      <c r="I57" s="85"/>
-      <c r="J57" s="85"/>
+      <c r="E57" s="104"/>
+      <c r="F57" s="83"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="83"/>
+      <c r="J57" s="83"/>
       <c r="K57" s="73"/>
       <c r="L57" s="73"/>
       <c r="M57" s="74"/>
@@ -4930,12 +4057,12 @@
       <c r="B58" s="73"/>
       <c r="C58" s="73"/>
       <c r="D58" s="73"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="85"/>
-      <c r="G58" s="85"/>
-      <c r="H58" s="85"/>
-      <c r="I58" s="85"/>
-      <c r="J58" s="85"/>
+      <c r="E58" s="104"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="83"/>
+      <c r="H58" s="83"/>
+      <c r="I58" s="83"/>
+      <c r="J58" s="83"/>
       <c r="K58" s="73"/>
       <c r="L58" s="73"/>
       <c r="M58" s="74"/>
@@ -4960,12 +4087,12 @@
       <c r="B59" s="73"/>
       <c r="C59" s="73"/>
       <c r="D59" s="73"/>
-      <c r="E59" s="106"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="85"/>
-      <c r="I59" s="85"/>
-      <c r="J59" s="85"/>
+      <c r="E59" s="104"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="83"/>
+      <c r="I59" s="83"/>
+      <c r="J59" s="83"/>
       <c r="K59" s="73"/>
       <c r="L59" s="73"/>
       <c r="M59" s="74"/>
@@ -33379,4 +32506,929 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="1" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="129"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="15"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="43"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="130"/>
+      <c r="G2" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="47"/>
+      <c r="N2" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="43"/>
+    </row>
+    <row r="3" spans="1:17" s="7" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="131"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="46">
+        <f>SUM(K4:K19)</f>
+        <v>217823.46153846153</v>
+      </c>
+      <c r="L3" s="46">
+        <f>SUM(L4:L19)</f>
+        <v>310516.15384615387</v>
+      </c>
+      <c r="M3" s="48"/>
+      <c r="N3" s="52">
+        <f>SUM(N4:N23)</f>
+        <v>108300</v>
+      </c>
+      <c r="O3" s="13">
+        <f>SUM(O4:O23)</f>
+        <v>300516.15384615387</v>
+      </c>
+      <c r="P3" s="13">
+        <f>SUM(P4:P23)</f>
+        <v>492183.07692307694</v>
+      </c>
+      <c r="Q3" s="44"/>
+    </row>
+    <row r="4" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="70">
+        <f>L4</f>
+        <v>92000</v>
+      </c>
+      <c r="E4" s="33">
+        <v>1</v>
+      </c>
+      <c r="F4" s="132"/>
+      <c r="G4" s="36">
+        <v>75000</v>
+      </c>
+      <c r="H4" s="65">
+        <v>92000</v>
+      </c>
+      <c r="I4" s="15">
+        <v>95000</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="35">
+        <f>L4*E4</f>
+        <v>92000</v>
+      </c>
+      <c r="L4" s="34">
+        <f>H4/E4</f>
+        <v>92000</v>
+      </c>
+      <c r="M4" s="30"/>
+      <c r="N4" s="41">
+        <f>O4</f>
+        <v>92000</v>
+      </c>
+      <c r="O4" s="14">
+        <f>L4</f>
+        <v>92000</v>
+      </c>
+      <c r="P4" s="9">
+        <f>O4</f>
+        <v>92000</v>
+      </c>
+      <c r="Q4" s="43"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="141">
+        <f>H5</f>
+        <v>10000</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" s="132"/>
+      <c r="G5" s="37">
+        <v>5000</v>
+      </c>
+      <c r="H5" s="142">
+        <v>10000</v>
+      </c>
+      <c r="I5" s="15">
+        <v>15000</v>
+      </c>
+      <c r="J5" s="30"/>
+      <c r="K5" s="35">
+        <f>H5</f>
+        <v>10000</v>
+      </c>
+      <c r="L5" s="35">
+        <f>H5</f>
+        <v>10000</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="43"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="70">
+        <f>L6</f>
+        <v>18000</v>
+      </c>
+      <c r="E6" s="128">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="132"/>
+      <c r="G6" s="37">
+        <v>10000</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="15">
+        <v>20000</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="35">
+        <f>L6*E6</f>
+        <v>14400</v>
+      </c>
+      <c r="L6" s="35">
+        <f>(I6-G6)*E6+G6</f>
+        <v>18000</v>
+      </c>
+      <c r="M6" s="30"/>
+      <c r="N6" s="42">
+        <f>G6</f>
+        <v>10000</v>
+      </c>
+      <c r="O6" s="14">
+        <f>L6</f>
+        <v>18000</v>
+      </c>
+      <c r="P6" s="9">
+        <f>I6</f>
+        <v>20000</v>
+      </c>
+      <c r="Q6" s="43"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="72">
+        <f>'Equity Valuation'!C26</f>
+        <v>24000</v>
+      </c>
+      <c r="E7" s="127">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="133"/>
+      <c r="G7" s="37">
+        <f>I7/4</f>
+        <v>36719.999999999993</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="15">
+        <f>'Equity Valuation'!J6</f>
+        <v>146879.99999999997</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="35">
+        <f>G7</f>
+        <v>36719.999999999993</v>
+      </c>
+      <c r="L7" s="35">
+        <f>I7*E7</f>
+        <v>73439.999999999985</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="42">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <f>L7</f>
+        <v>73439.999999999985</v>
+      </c>
+      <c r="P7" s="9">
+        <f>I7</f>
+        <v>146879.99999999997</v>
+      </c>
+      <c r="Q7" s="43"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="71">
+        <f>'Equity Valuation'!C29</f>
+        <v>24000</v>
+      </c>
+      <c r="E8" s="127">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="133"/>
+      <c r="G8" s="37">
+        <f>I8/4</f>
+        <v>49140</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="15">
+        <f>'Equity Valuation'!K6</f>
+        <v>196560</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="35">
+        <f>G8</f>
+        <v>49140</v>
+      </c>
+      <c r="L8" s="35">
+        <f>I8*E8</f>
+        <v>98280</v>
+      </c>
+      <c r="M8" s="30"/>
+      <c r="N8" s="42">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <f>L8</f>
+        <v>98280</v>
+      </c>
+      <c r="P8" s="9">
+        <f>I8</f>
+        <v>196560</v>
+      </c>
+      <c r="Q8" s="43"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="31">
+        <f>H9</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0.66</v>
+      </c>
+      <c r="F9" s="134"/>
+      <c r="G9" s="38">
+        <v>2</v>
+      </c>
+      <c r="H9" s="22">
+        <v>3</v>
+      </c>
+      <c r="I9" s="21">
+        <v>6</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="35">
+        <f t="shared" ref="K9:K19" si="0">L9*E9</f>
+        <v>4188.4615384615381</v>
+      </c>
+      <c r="L9" s="35">
+        <f>(L4+L6)/52*H9</f>
+        <v>6346.1538461538457</v>
+      </c>
+      <c r="M9" s="30"/>
+      <c r="N9" s="42">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <f>L9</f>
+        <v>6346.1538461538457</v>
+      </c>
+      <c r="P9" s="9">
+        <f>D4/52*H9</f>
+        <v>5307.6923076923076</v>
+      </c>
+      <c r="Q9" s="43"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="70">
+        <f>H10</f>
+        <v>500</v>
+      </c>
+      <c r="E10" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="134"/>
+      <c r="G10" s="64">
+        <v>400</v>
+      </c>
+      <c r="H10" s="65">
+        <v>500</v>
+      </c>
+      <c r="I10" s="66">
+        <v>600</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="35">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="L10" s="35">
+        <f t="shared" ref="L10:L18" si="1">O10</f>
+        <v>250</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="42">
+        <f>G10*E10</f>
+        <v>200</v>
+      </c>
+      <c r="O10" s="9">
+        <f>H10*E$10</f>
+        <v>250</v>
+      </c>
+      <c r="P10" s="9">
+        <f>I10*E10</f>
+        <v>300</v>
+      </c>
+      <c r="Q10" s="43"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="70">
+        <f>H11</f>
+        <v>2000</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="134"/>
+      <c r="G11" s="64">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="65">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="66">
+        <v>3000</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="35">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="L11" s="35">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="M11" s="30"/>
+      <c r="N11" s="42">
+        <f>G11*E11</f>
+        <v>500</v>
+      </c>
+      <c r="O11" s="9">
+        <f>H11*E$10</f>
+        <v>1000</v>
+      </c>
+      <c r="P11" s="9">
+        <f>I11*E11</f>
+        <v>1500</v>
+      </c>
+      <c r="Q11" s="43"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="70">
+        <f>H12</f>
+        <v>1800</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="134"/>
+      <c r="G12" s="64">
+        <v>1000</v>
+      </c>
+      <c r="H12" s="65">
+        <v>1800</v>
+      </c>
+      <c r="I12" s="66">
+        <v>3000</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="35">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="L12" s="35">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="M12" s="30"/>
+      <c r="N12" s="42">
+        <f>G12*E12</f>
+        <v>500</v>
+      </c>
+      <c r="O12" s="9">
+        <f>H12*E$10</f>
+        <v>900</v>
+      </c>
+      <c r="P12" s="9">
+        <f>I12*E12</f>
+        <v>1500</v>
+      </c>
+      <c r="Q12" s="43"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="70">
+        <f>K13</f>
+        <v>4600</v>
+      </c>
+      <c r="E13" s="32">
+        <v>1</v>
+      </c>
+      <c r="F13" s="129"/>
+      <c r="G13" s="39">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="J13" s="30"/>
+      <c r="K13" s="35">
+        <f t="shared" si="0"/>
+        <v>4600</v>
+      </c>
+      <c r="L13" s="35">
+        <f t="shared" si="1"/>
+        <v>4600</v>
+      </c>
+      <c r="M13" s="30"/>
+      <c r="N13" s="42">
+        <f>$D$4*G13</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
+        <f>$D$4*H13</f>
+        <v>4600</v>
+      </c>
+      <c r="P13" s="9">
+        <f>$D$4*I13</f>
+        <v>5520</v>
+      </c>
+      <c r="Q13" s="43"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="135">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="32">
+        <v>1</v>
+      </c>
+      <c r="F14" s="129"/>
+      <c r="G14" s="40">
+        <v>400</v>
+      </c>
+      <c r="H14" s="26">
+        <v>550</v>
+      </c>
+      <c r="I14" s="25">
+        <v>800</v>
+      </c>
+      <c r="J14" s="30"/>
+      <c r="K14" s="35">
+        <f t="shared" si="0"/>
+        <v>3300</v>
+      </c>
+      <c r="L14" s="35">
+        <f t="shared" si="1"/>
+        <v>3300</v>
+      </c>
+      <c r="M14" s="30"/>
+      <c r="N14" s="42">
+        <f>G14*12*$D$14</f>
+        <v>2400</v>
+      </c>
+      <c r="O14" s="9">
+        <f>H14*12*$D$14</f>
+        <v>3300</v>
+      </c>
+      <c r="P14" s="9">
+        <f>I14*12*$D$14</f>
+        <v>4800</v>
+      </c>
+      <c r="Q14" s="43"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="70">
+        <f>H15</f>
+        <v>75</v>
+      </c>
+      <c r="E15" s="32">
+        <v>1</v>
+      </c>
+      <c r="F15" s="129"/>
+      <c r="G15" s="67">
+        <v>50</v>
+      </c>
+      <c r="H15" s="68">
+        <v>75</v>
+      </c>
+      <c r="I15" s="69">
+        <v>100</v>
+      </c>
+      <c r="J15" s="30"/>
+      <c r="K15" s="35">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="L15" s="35">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="M15" s="30"/>
+      <c r="N15" s="42">
+        <f>G15*E15*12</f>
+        <v>600</v>
+      </c>
+      <c r="O15" s="9">
+        <f>H15*E$10*12</f>
+        <v>450</v>
+      </c>
+      <c r="P15" s="9">
+        <f>I15*E15*12</f>
+        <v>1200</v>
+      </c>
+      <c r="Q15" s="43"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="70">
+        <f>H16</f>
+        <v>125</v>
+      </c>
+      <c r="E16" s="32">
+        <v>1</v>
+      </c>
+      <c r="F16" s="129"/>
+      <c r="G16" s="67">
+        <v>75</v>
+      </c>
+      <c r="H16" s="68">
+        <v>125</v>
+      </c>
+      <c r="I16" s="69">
+        <v>200</v>
+      </c>
+      <c r="J16" s="30"/>
+      <c r="K16" s="35">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="L16" s="35">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+      <c r="M16" s="30"/>
+      <c r="N16" s="42">
+        <f>G16*E16*12</f>
+        <v>900</v>
+      </c>
+      <c r="O16" s="9">
+        <f>H16*E$10*12</f>
+        <v>750</v>
+      </c>
+      <c r="P16" s="9">
+        <f>I16*E16*12</f>
+        <v>2400</v>
+      </c>
+      <c r="Q16" s="43"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="70">
+        <f>H17</f>
+        <v>200</v>
+      </c>
+      <c r="E17" s="32">
+        <v>1</v>
+      </c>
+      <c r="F17" s="129"/>
+      <c r="G17" s="67">
+        <v>100</v>
+      </c>
+      <c r="H17" s="68">
+        <v>200</v>
+      </c>
+      <c r="I17" s="69">
+        <v>300</v>
+      </c>
+      <c r="J17" s="30"/>
+      <c r="K17" s="35">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="L17" s="35">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="M17" s="30"/>
+      <c r="N17" s="42">
+        <f>G17*E17*12</f>
+        <v>1200</v>
+      </c>
+      <c r="O17" s="9">
+        <f>H17*E$10*12</f>
+        <v>1200</v>
+      </c>
+      <c r="P17" s="9">
+        <f>I17*E17*12</f>
+        <v>3600</v>
+      </c>
+      <c r="Q17" s="43"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="31">
+        <f>H18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="134"/>
+      <c r="G18" s="38">
+        <v>0</v>
+      </c>
+      <c r="H18" s="22">
+        <f>I18*E18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
+        <v>6</v>
+      </c>
+      <c r="J18" s="30"/>
+      <c r="K18" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="30"/>
+      <c r="N18" s="42">
+        <f>$H$4/52*G18</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="14">
+        <f>$H$4/52*H18</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="9">
+        <f>$H$4/52*I18</f>
+        <v>10615.384615384615</v>
+      </c>
+      <c r="Q18" s="43"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="129"/>
+      <c r="G19" s="64">
+        <v>0</v>
+      </c>
+      <c r="H19" s="65">
+        <v>0</v>
+      </c>
+      <c r="I19" s="66">
+        <v>0</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="K19" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="35">
+        <f>H19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="30"/>
+      <c r="N19" s="42">
+        <f>G19</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="9">
+        <f>H19</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="9">
+        <f>I19</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="43"/>
+    </row>
+    <row r="20" spans="1:17" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="43"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E23" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>